<commit_message>
Latest Code with Append API's
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nawaz\Desktop\results\hauna\New Result Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E687495-DFA3-45B6-AC3D-A5AFCDCCE75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD02C45-E0A3-4D25-9A69-85FE581808EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>